<commit_message>
Finaliza la jerarquía de dependencias de los combos. Se corrige bug que dejaba el plazo en 12 meses cuando se seleccionaba indemnización vf a dos años. (Se agregó al event handler el manejo de [SELECCION_INDEMN_AÑO1])
</commit_message>
<xml_diff>
--- a/Events Doc/Jerarquía de Combos.xlsx
+++ b/Events Doc/Jerarquía de Combos.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Servas\Documents\Repos\AutoEstrene\Events Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="19152" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t>Producto</t>
   </si>
@@ -82,14 +87,14 @@
     <t>Réplicas/Cálculo</t>
   </si>
   <si>
-    <t>Valor Garantía Extendida</t>
+    <t>Valor Garantía Extendida ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,17 +131,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -183,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +229,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,6 +281,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,19 +474,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:E52"/>
+  <dimension ref="B1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="5" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="5" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -448,206 +498,209 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
-      <c r="C3" t="s">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
-      <c r="C4" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D47" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="C9" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="C22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="C27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="C31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="B34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="B36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="C37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3">
-      <c r="C38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="B44" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="B48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="B52" t="s">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
         <v>20</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D51" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hace un arbol con la jerarquía de combos.
</commit_message>
<xml_diff>
--- a/Events Doc/Jerarquía de Combos.xlsx
+++ b/Events Doc/Jerarquía de Combos.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Servas\Documents\Repos\AutoEstrene\Events Doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="19152" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arbol" sheetId="1" r:id="rId1"/>
+    <sheet name="Lista" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Arbol!$B$1:$G$20</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
   <si>
     <t>Producto</t>
   </si>
@@ -88,13 +87,19 @@
   </si>
   <si>
     <t>Valor Garantía Extendida ?</t>
+  </si>
+  <si>
+    <t>Calculo Seguro</t>
+  </si>
+  <si>
+    <t>Arbol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +115,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,12 +164,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,6 +197,785 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Elbow Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="571500"/>
+          <a:ext cx="762000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Elbow Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="571500"/>
+          <a:ext cx="762000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Elbow Connector 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="571500"/>
+          <a:ext cx="762000" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Elbow Connector 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7620000" y="1143000"/>
+          <a:ext cx="762000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Elbow Connector 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7620000" y="1143000"/>
+          <a:ext cx="762000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Elbow Connector 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="2286000"/>
+          <a:ext cx="762000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Elbow Connector 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="2286000"/>
+          <a:ext cx="762000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Elbow Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="2286000"/>
+          <a:ext cx="762000" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Elbow Connector 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9906000" y="2857500"/>
+          <a:ext cx="762000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Elbow Connector 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="2095500"/>
+          <a:ext cx="762000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Elbow Connector 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7620000" y="1905000"/>
+          <a:ext cx="762000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Elbow Connector 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="1714500"/>
+          <a:ext cx="762000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Elbow Connector 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7620000" y="3238500"/>
+          <a:ext cx="762000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>350384</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>350384</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Connector 32"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="578304" y="2204357"/>
+          <a:ext cx="0" cy="2279197"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>353785</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Connector 38"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="581705" y="3799795"/>
+          <a:ext cx="350385" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>353784</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>224519</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>704169</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>224519</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Connector 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="581704" y="4252233"/>
+          <a:ext cx="350385" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>353784</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>704169</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Connector 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="581704" y="4483554"/>
+          <a:ext cx="350385" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -197,7 +1021,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,27 +1053,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,24 +1087,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,19 +1262,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:E51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="5" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
+      <c r="A1" s="6"/>
+      <c r="B1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="3" spans="1:7" ht="18" customHeight="1">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" customHeight="1">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" customHeight="1">
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" customHeight="1">
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="18" customHeight="1">
+      <c r="D8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="18" customHeight="1">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" customHeight="1">
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" customHeight="1">
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" customHeight="1">
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1">
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" customHeight="1">
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" customHeight="1">
+      <c r="G16" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="18" customHeight="1">
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="18" customHeight="1">
+      <c r="D18" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="18" customHeight="1">
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="18" customHeight="1">
+      <c r="C20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="10"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.59055118110236204" right="0.59055118110236204" top="0.59055118110236204" bottom="0.59055118110236204" header="0.39370078740157499" footer="0.39370078740157499"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LArchivo: &amp;F
+Página &amp;P de &amp;N&amp;RHoja: &amp;A
+&amp;D - &amp;T</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="B1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="4" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -496,58 +1412,57 @@
       <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4">
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4">
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
+    <row r="7" spans="2:4">
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="2:4">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4">
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
+    <row r="11" spans="2:4">
+      <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -555,65 +1470,65 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4">
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4">
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="2" t="s">
+    <row r="16" spans="2:4">
+      <c r="C16" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3">
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="2" t="s">
+    <row r="18" spans="2:3">
+      <c r="C18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3">
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="2" t="s">
+    <row r="20" spans="2:3">
+      <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C21" s="2" t="s">
+    <row r="21" spans="2:3">
+      <c r="C21" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3">
       <c r="C24" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3">
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3">
       <c r="B27" t="s">
         <v>11</v>
       </c>
@@ -621,66 +1536,66 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3">
       <c r="B29" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3">
       <c r="C30" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C31" s="2" t="s">
+    <row r="31" spans="2:3">
+      <c r="C31" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4">
       <c r="B33" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4">
       <c r="B35" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4">
       <c r="B37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4">
       <c r="B39" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4">
       <c r="B41" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4">
       <c r="B43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
+    <row r="45" spans="2:4">
+      <c r="B45" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4">
       <c r="B47" t="s">
         <v>1</v>
       </c>
@@ -688,7 +1603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4">
       <c r="B49" t="s">
         <v>7</v>
       </c>
@@ -696,7 +1611,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4">
       <c r="B51" t="s">
         <v>20</v>
       </c>

</xml_diff>